<commit_message>
change the name translation to find mistakes
</commit_message>
<xml_diff>
--- a/Conversion-Script/Variable_Reference/Variable_name_IAMC.xlsx
+++ b/Conversion-Script/Variable_Reference/Variable_name_IAMC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdGeeds\Documents\IAMC-format\IAMC_format\Conversion-Script\Variable_Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DF1CE7-F2F4-4696-888E-A9C7C109EE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4819F51C-1C8D-4260-A906-E4F0F3E89518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="389">
   <si>
     <t>IAMC_variable</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Gt/Year</t>
   </si>
   <si>
-    <t>Emissions|CO2eq|Per capita</t>
-  </si>
-  <si>
     <t>t/(Year*person)</t>
   </si>
   <si>
@@ -288,9 +285,6 @@
     <t>number_households_by_type_EU27</t>
   </si>
   <si>
-    <t>Population|Urban|Share</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -351,9 +345,6 @@
     <t>DB_LABOUR_COMPENSATION</t>
   </si>
   <si>
-    <t>Value Added|Net operating surplus</t>
-  </si>
-  <si>
     <t>DB_NET_OPERATING_SURPLUS</t>
   </si>
   <si>
@@ -453,15 +444,9 @@
     <t>unemployment_rate</t>
   </si>
   <si>
-    <t>Revenue|government</t>
-  </si>
-  <si>
     <t>government_revenue</t>
   </si>
   <si>
-    <t>Expenditure|government</t>
-  </si>
-  <si>
     <t>government_expenditure</t>
   </si>
   <si>
@@ -522,24 +507,15 @@
     <t>DB_HH_SAVINGS_NOMINAL</t>
   </si>
   <si>
-    <t>GDP|Country|Per capita</t>
-  </si>
-  <si>
     <t>DB_GDP_PER_CAPITA</t>
   </si>
   <si>
     <t>dollars_2015/person</t>
   </si>
   <si>
-    <t>Revenue|Households|Disposable per capita</t>
-  </si>
-  <si>
     <t>DB_DISPOSABLE_INCOME_PER_CAPITA</t>
   </si>
   <si>
-    <t>Households|Consumer Price Index</t>
-  </si>
-  <si>
     <t>consumer_price_index</t>
   </si>
   <si>
@@ -588,9 +564,6 @@
     <t>disposable_income_real</t>
   </si>
   <si>
-    <t>Expenditure|household|Real</t>
-  </si>
-  <si>
     <t>consumption_COICOP_real</t>
   </si>
   <si>
@@ -711,21 +684,12 @@
     <t>stationary_electrolyzer_capacity_stock</t>
   </si>
   <si>
-    <t>Final Energy|Electricity|Renewable|Share</t>
-  </si>
-  <si>
     <t>shares_RES_in_FE</t>
   </si>
   <si>
-    <t>Final Energy|Renewable|Share</t>
-  </si>
-  <si>
     <t>share_FE_RES_vs_total_FE</t>
   </si>
   <si>
-    <t>Primary Energy|Renewable|Share</t>
-  </si>
-  <si>
     <t>share_RES_in_PE</t>
   </si>
   <si>
@@ -867,15 +831,9 @@
     <t>total_FE_including_trade_per_capita</t>
   </si>
   <si>
-    <t>Capacity|Electricity|Storage|Battery Electric Vehicles with SC</t>
-  </si>
-  <si>
     <t>power_charge_vehicles_with_SC</t>
   </si>
   <si>
-    <t>Capacity|Electricity|Power|Battery Electric Vehicles with SC</t>
-  </si>
-  <si>
     <t>capacity_charge_vehicles_with_SC</t>
   </si>
   <si>
@@ -888,9 +846,6 @@
     <t>total_electrified_vehicles_batteries_power_required</t>
   </si>
   <si>
-    <t>Capacity|Electricity|Storage|Battery Electric Vehicles</t>
-  </si>
-  <si>
     <t>transport_electrified_vehicle_batteries_capacity</t>
   </si>
   <si>
@@ -1119,9 +1074,6 @@
     <t>N2O_emissions_agriculture</t>
   </si>
   <si>
-    <t>Resource|Consumption per capita</t>
-  </si>
-  <si>
     <t>materials_consumption_per_capita</t>
   </si>
   <si>
@@ -1186,26 +1138,91 @@
   </si>
   <si>
     <t>Capacity|Electricity</t>
+  </si>
+  <si>
+    <t>Expenditure|Household|Real</t>
+  </si>
+  <si>
+    <t>Expenditure|Government</t>
+  </si>
+  <si>
+    <t>Revenue|Government</t>
+  </si>
+  <si>
+    <t>GDP|Country|Per Capita</t>
+  </si>
+  <si>
+    <t>Primary Energy|Renewable [Share]</t>
+  </si>
+  <si>
+    <t>Final Energy|Renewable [Share]</t>
+  </si>
+  <si>
+    <t>Final Energy|Electricity|Renewable [Share]</t>
+  </si>
+  <si>
+    <t>Households|Consumer Price [index]</t>
+  </si>
+  <si>
+    <t>Revenue|Households|Disposable [per capita]</t>
+  </si>
+  <si>
+    <t>Value Added|Net Operating Surplus</t>
+  </si>
+  <si>
+    <t>Population|Urban [Share]</t>
+  </si>
+  <si>
+    <t>Emissions|CO2eq [Per capita]</t>
+  </si>
+  <si>
+    <t>Resource|Consumption [per capita]</t>
+  </si>
+  <si>
+    <t>Final Energy|Transportation|Smart Charging|Electricity</t>
+  </si>
+  <si>
+    <t>Capacity|Electricity|Storage|Battery Capacity|Electric Vehicules|Smart Charging</t>
+  </si>
+  <si>
+    <t>Capacity|Electricity|Storage|Battery Capacity|Electric Vehicles</t>
+  </si>
+  <si>
+    <t>Price Adjusted|Primary Energy</t>
+  </si>
+  <si>
+    <t>Primary Energy|Commodity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1220,12 +1237,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1542,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1604,8 +1631,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
+      <c r="A5" s="6" t="s">
+        <v>387</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
@@ -1695,111 +1722,111 @@
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>31</v>
@@ -1807,13 +1834,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>31</v>
@@ -1821,13 +1848,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>31</v>
@@ -1835,13 +1862,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>31</v>
@@ -1849,13 +1876,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>31</v>
@@ -1863,139 +1890,139 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="D30" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="D32" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>14</v>
@@ -2003,321 +2030,321 @@
     </row>
     <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>108</v>
+        <v>380</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>14</v>
@@ -2325,55 +2352,55 @@
     </row>
     <row r="57" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>142</v>
+        <v>373</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>144</v>
+        <v>372</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>14</v>
@@ -2381,139 +2408,139 @@
     </row>
     <row r="61" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>165</v>
+        <v>374</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>168</v>
+        <v>379</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>170</v>
+        <v>378</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>14</v>
@@ -2521,203 +2548,203 @@
     </row>
     <row r="71" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>187</v>
+        <v>371</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="1" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="1" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="1" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>14</v>
@@ -2725,11 +2752,11 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="1" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>14</v>
@@ -2737,23 +2764,23 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="1" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>14</v>
@@ -2761,119 +2788,119 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="1" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="1" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="1" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>228</v>
+        <v>377</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>14</v>
@@ -2881,13 +2908,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>230</v>
+        <v>376</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>14</v>
@@ -2895,13 +2922,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>232</v>
+        <v>375</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>14</v>
@@ -2909,27 +2936,27 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>14</v>
@@ -2937,11 +2964,11 @@
     </row>
     <row r="102" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" s="1" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>14</v>
@@ -2949,111 +2976,111 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>14</v>
@@ -3061,25 +3088,25 @@
     </row>
     <row r="111" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" s="1" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>14</v>
@@ -3087,23 +3114,23 @@
     </row>
     <row r="113" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" s="1" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" s="1" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>14</v>
@@ -3111,11 +3138,11 @@
     </row>
     <row r="115" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" s="1" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>14</v>
@@ -3123,23 +3150,23 @@
     </row>
     <row r="116" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" s="1" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" s="1" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>14</v>
@@ -3147,11 +3174,11 @@
     </row>
     <row r="118" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" s="1" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>14</v>
@@ -3159,225 +3186,225 @@
     </row>
     <row r="119" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" s="1" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" s="1" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>4</v>
+      <c r="A121" s="6" t="s">
+        <v>388</v>
       </c>
       <c r="B121" s="2"/>
       <c r="C121" s="1" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="D121" s="2"/>
     </row>
     <row r="122" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="B122" s="2"/>
       <c r="C122" s="1" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" s="1" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>280</v>
+        <v>385</v>
       </c>
       <c r="B124" s="2"/>
       <c r="C124" s="1" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>282</v>
+        <v>384</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B126" s="2"/>
-      <c r="C126" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>225</v>
+      <c r="A126" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B126" s="4"/>
+      <c r="C126" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>287</v>
+        <v>386</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" s="1" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" s="1" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="B130" s="2"/>
       <c r="C130" s="1" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="B131" s="2"/>
       <c r="C131" s="1" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="B132" s="2"/>
       <c r="C132" s="1" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="B133" s="2"/>
       <c r="C133" s="1" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" s="1" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" s="1" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B136" s="2"/>
       <c r="C136" s="1" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="B137" s="2"/>
       <c r="C137" s="1" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>14</v>
@@ -3385,119 +3412,119 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="B138" s="2"/>
       <c r="C138" s="1" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="B139" s="2"/>
       <c r="C139" s="1" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="B140" s="2"/>
       <c r="C140" s="1" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" s="1" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" s="1" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" s="1" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" s="1" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" s="1" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="B146" s="2"/>
       <c r="C146" s="1" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="B147" s="2"/>
       <c r="C147" s="1" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>14</v>
@@ -3505,11 +3532,11 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="B148" s="2"/>
       <c r="C148" s="1" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>14</v>
@@ -3517,11 +3544,11 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="B149" s="2"/>
       <c r="C149" s="1" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>14</v>
@@ -3529,11 +3556,11 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="B150" s="2"/>
       <c r="C150" s="1" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>14</v>
@@ -3541,23 +3568,23 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="B151" s="2"/>
       <c r="C151" s="1" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="B152" s="2"/>
       <c r="C152" s="1" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>14</v>
@@ -3565,11 +3592,11 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="B153" s="2"/>
       <c r="C153" s="1" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>14</v>
@@ -3577,11 +3604,11 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="B154" s="2"/>
       <c r="C154" s="1" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>14</v>
@@ -3589,11 +3616,11 @@
     </row>
     <row r="155" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="B155" s="2"/>
       <c r="C155" s="1" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>14</v>
@@ -3601,149 +3628,149 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="B156" s="2"/>
       <c r="C156" s="1" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="B158" s="2"/>
       <c r="C158" s="1" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="B159" s="2"/>
       <c r="C159" s="1" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" s="1" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>364</v>
+        <v>383</v>
       </c>
       <c r="B161" s="2"/>
       <c r="C161" s="1" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" s="1" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" s="1" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" s="1" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="1" t="s">
-        <v>380</v>
+      <c r="A167" s="5" t="s">
+        <v>364</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" s="1" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>14</v>
@@ -3751,7 +3778,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
change naming of variable for the first dictionnary
</commit_message>
<xml_diff>
--- a/Conversion-Script/Variable_Reference/Variable_name_IAMC.xlsx
+++ b/Conversion-Script/Variable_Reference/Variable_name_IAMC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdGeeds\Documents\IAMC-format\IAMC_format\Conversion-Script\Variable_Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4819F51C-1C8D-4260-A906-E4F0F3E89518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1926A5-0C12-43C3-972E-16C38F466808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="388">
   <si>
     <t>IAMC_variable</t>
   </si>
@@ -63,9 +63,6 @@
     <t>fuel_price_by_PROTRA_9R_adjusted</t>
   </si>
   <si>
-    <t>Index Price|Final Energy</t>
-  </si>
-  <si>
     <t>price_final_energy</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>total_CO2e_emissions_per_capita_9R</t>
   </si>
   <si>
-    <t>Emissions|Per capita</t>
-  </si>
-  <si>
     <t>GHG_emissions_per_capita_9R</t>
   </si>
   <si>
@@ -147,9 +141,6 @@
     <t>DegreesC</t>
   </si>
   <si>
-    <t>Sea level|Region|Mean rise</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
@@ -270,18 +261,12 @@
     <t>total_population_over_15</t>
   </si>
   <si>
-    <t>Households|number</t>
-  </si>
-  <si>
     <t>number_households_nonEU</t>
   </si>
   <si>
     <t>households</t>
   </si>
   <si>
-    <t>Households|type|number</t>
-  </si>
-  <si>
     <t>number_households_by_type_EU27</t>
   </si>
   <si>
@@ -519,42 +504,27 @@
     <t>consumer_price_index</t>
   </si>
   <si>
-    <t>Value|Added Real</t>
-  </si>
-  <si>
     <t>gross_value_added_real</t>
   </si>
   <si>
     <t>Mdollars 2015/Year</t>
   </si>
   <si>
-    <t>Value|GDP deflator</t>
-  </si>
-  <si>
     <t>gross_domestic_product_deflator</t>
   </si>
   <si>
     <t>Mdollars/Mdollars 2015</t>
   </si>
   <si>
-    <t>Value|GDP real</t>
-  </si>
-  <si>
     <t>gross_domestic_product_real_supply_side</t>
   </si>
   <si>
     <t>Mdollars_2015/Year</t>
   </si>
   <si>
-    <t>Value|Final Demand real|Taxes on products</t>
-  </si>
-  <si>
     <t>taxes_products_final_demand_real</t>
   </si>
   <si>
-    <t>Value|GDP real|Taxes products</t>
-  </si>
-  <si>
     <t>taxes_products_by_sector_real</t>
   </si>
   <si>
@@ -579,9 +549,6 @@
     <t>final_demand_dometic_in_basic_prices_real_by_component</t>
   </si>
   <si>
-    <t>Energy Intensity</t>
-  </si>
-  <si>
     <t>final_energy_intensities_by_sector_and_FE</t>
   </si>
   <si>
@@ -600,9 +567,6 @@
     <t>final_energy_demand_by_FE_9R</t>
   </si>
   <si>
-    <t>Intensity|Final Energy|Non-Energy Use</t>
-  </si>
-  <si>
     <t>non_energy_use_intensities_by_sector_and_FE</t>
   </si>
   <si>
@@ -651,9 +615,6 @@
     <t>PROSUP_storage_losses</t>
   </si>
   <si>
-    <t>Final Energy|Flexibility options</t>
-  </si>
-  <si>
     <t>PROSUP_flexibility_technologies</t>
   </si>
   <si>
@@ -774,18 +735,12 @@
     <t>efficiences_PV_technology_panels</t>
   </si>
   <si>
-    <t>Intensity|Primary Energy vs GDP</t>
-  </si>
-  <si>
     <t>PE_GDP_intensity</t>
   </si>
   <si>
     <t>TJ/Mdollars_2015</t>
   </si>
   <si>
-    <t>Intensity|Primary Energy vs GDP|Annual change</t>
-  </si>
-  <si>
     <t>annual_PE_GDP_intensity_change_rate</t>
   </si>
   <si>
@@ -915,18 +870,12 @@
     <t>share_curtailment_TO_elec</t>
   </si>
   <si>
-    <t>Intensity|Emissions</t>
-  </si>
-  <si>
     <t>GHG_intensity_of_final_energy</t>
   </si>
   <si>
     <t>Mt/EJ</t>
   </si>
   <si>
-    <t>Intensity|Emissions|CO2eq</t>
-  </si>
-  <si>
     <t>CO2e_intensity_of_final_energy</t>
   </si>
   <si>
@@ -984,27 +933,15 @@
     <t>total_sea_area_use_PROTRA</t>
   </si>
   <si>
-    <t>EROI|static|PV</t>
-  </si>
-  <si>
     <t>EROIst_PV_technologies</t>
   </si>
   <si>
-    <t>EROI|final|PV</t>
-  </si>
-  <si>
     <t>EROIfinal_PV_technologies</t>
   </si>
   <si>
-    <t>EROI|static</t>
-  </si>
-  <si>
     <t>EROIst_PROTRA</t>
   </si>
   <si>
-    <t>EROI|dynamic</t>
-  </si>
-  <si>
     <t>dynEROIst_PROTRA</t>
   </si>
   <si>
@@ -1017,24 +954,15 @@
     <t>Year</t>
   </si>
   <si>
-    <t>EROI|static|Global</t>
-  </si>
-  <si>
     <t>global_EROIst_system</t>
   </si>
   <si>
     <t>EROIst_system</t>
   </si>
   <si>
-    <t>EROI|static|Electric Vehicles</t>
-  </si>
-  <si>
     <t>total_ESOIst_electrified_vehicles</t>
   </si>
   <si>
-    <t>EROI|static|Storage|Pumped Hydropower plants</t>
-  </si>
-  <si>
     <t>ESOIst_PHS</t>
   </si>
   <si>
@@ -1128,15 +1056,6 @@
     <t>Energy|Supply|Storage|Losses Vs Transformation Output [Share]</t>
   </si>
   <si>
-    <t>Final Energy|Net [per capita]</t>
-  </si>
-  <si>
-    <t>Final Energy [per capita]</t>
-  </si>
-  <si>
-    <t>Primary Energy [per capita]</t>
-  </si>
-  <si>
     <t>Capacity|Electricity</t>
   </si>
   <si>
@@ -1149,9 +1068,6 @@
     <t>Revenue|Government</t>
   </si>
   <si>
-    <t>GDP|Country|Per Capita</t>
-  </si>
-  <si>
     <t>Primary Energy|Renewable [Share]</t>
   </si>
   <si>
@@ -1164,21 +1080,12 @@
     <t>Households|Consumer Price [index]</t>
   </si>
   <si>
-    <t>Revenue|Households|Disposable [per capita]</t>
-  </si>
-  <si>
     <t>Value Added|Net Operating Surplus</t>
   </si>
   <si>
     <t>Population|Urban [Share]</t>
   </si>
   <si>
-    <t>Emissions|CO2eq [Per capita]</t>
-  </si>
-  <si>
-    <t>Resource|Consumption [per capita]</t>
-  </si>
-  <si>
     <t>Final Energy|Transportation|Smart Charging|Electricity</t>
   </si>
   <si>
@@ -1192,6 +1099,96 @@
   </si>
   <si>
     <t>Primary Energy|Commodity</t>
+  </si>
+  <si>
+    <t>Sea level|Regional Mean rise</t>
+  </si>
+  <si>
+    <t>Emissions|CO2eq[per capita]</t>
+  </si>
+  <si>
+    <t>GDP|Country[per capita]</t>
+  </si>
+  <si>
+    <t>Revenue|Households|Disposable[per capita]</t>
+  </si>
+  <si>
+    <t>Final Energy|Net[per capita]</t>
+  </si>
+  <si>
+    <t>Final Energy[per capita]</t>
+  </si>
+  <si>
+    <t>Primary Energy[per capita]</t>
+  </si>
+  <si>
+    <t>Resource|Consumption[per capita]</t>
+  </si>
+  <si>
+    <t>Households|Number</t>
+  </si>
+  <si>
+    <t>Final Energy[intensity]</t>
+  </si>
+  <si>
+    <t>Final Energy|Non-Energy Use[intensity]</t>
+  </si>
+  <si>
+    <t>Emissions[intensity]</t>
+  </si>
+  <si>
+    <t>Emissions|CO2eq[intensity]</t>
+  </si>
+  <si>
+    <t>EROI|Static|PV</t>
+  </si>
+  <si>
+    <t>EROI|Final|PV</t>
+  </si>
+  <si>
+    <t>EROI|Dynamic</t>
+  </si>
+  <si>
+    <t>EROI|Static</t>
+  </si>
+  <si>
+    <t>EROI|Static|Global</t>
+  </si>
+  <si>
+    <t>ESOI|Static|Storage|Pumped Hydropower Plants</t>
+  </si>
+  <si>
+    <t>ESOI|Static</t>
+  </si>
+  <si>
+    <t>Price|Final Energy[index]</t>
+  </si>
+  <si>
+    <t>Emissions[per capita]</t>
+  </si>
+  <si>
+    <t>Value Added|Real</t>
+  </si>
+  <si>
+    <t>Value|GDP Real</t>
+  </si>
+  <si>
+    <t>Value|GDP Deflator</t>
+  </si>
+  <si>
+    <t>Value|GDP Real|Taxes on Products</t>
+  </si>
+  <si>
+    <t>Value|Final Demand real|Taxes on Products</t>
+  </si>
+  <si>
+    <t>Final Energy|Flexibility Options</t>
+  </si>
+  <si>
+    <t>Primary Energy Intensity|GDP</t>
+  </si>
+  <si>
+    <t>Primary Energy Intensity|GDP[Annual change]</t>
   </si>
 </sst>
 </file>
@@ -1569,8 +1566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1632,7 +1629,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>387</v>
+        <v>356</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
@@ -1644,2136 +1641,2136 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>378</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>382</v>
+        <v>359</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>379</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>358</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="D20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="D29" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>81</v>
+        <v>366</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>84</v>
+        <v>366</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>381</v>
+        <v>352</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>373</v>
+        <v>346</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>372</v>
+        <v>345</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>378</v>
+        <v>350</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>164</v>
+        <v>380</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>167</v>
+        <v>382</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>170</v>
+        <v>381</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>173</v>
+        <v>384</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>175</v>
+        <v>383</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>371</v>
+        <v>344</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>184</v>
+        <v>367</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="1" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="1" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>193</v>
+        <v>368</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="1" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="1" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="1" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" s="1" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>208</v>
+        <v>385</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="1" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="1" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="1" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>377</v>
+        <v>349</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>376</v>
+        <v>348</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>375</v>
+        <v>347</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" s="1" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>370</v>
+        <v>343</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" s="1" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>249</v>
+        <v>386</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" s="1" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>252</v>
+        <v>387</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" s="1" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" s="1" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" s="1" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" s="1" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" s="1" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
-        <v>388</v>
+        <v>357</v>
       </c>
       <c r="B121" s="2"/>
       <c r="C121" s="1" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="D121" s="2"/>
     </row>
     <row r="122" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="B122" s="2"/>
       <c r="C122" s="1" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" s="1" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>385</v>
+        <v>354</v>
       </c>
       <c r="B124" s="2"/>
       <c r="C124" s="1" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>384</v>
+        <v>353</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" s="1" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="B126" s="4"/>
       <c r="C126" s="3" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>386</v>
+        <v>355</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" s="1" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" s="1" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="B130" s="2"/>
       <c r="C130" s="1" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="B131" s="2"/>
       <c r="C131" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="B132" s="2"/>
       <c r="C132" s="1" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="B133" s="2"/>
       <c r="C133" s="1" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" s="1" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" s="1" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="B136" s="2"/>
       <c r="C136" s="1" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="B137" s="2"/>
       <c r="C137" s="1" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>296</v>
+        <v>369</v>
       </c>
       <c r="B138" s="2"/>
       <c r="C138" s="1" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>299</v>
+        <v>370</v>
       </c>
       <c r="B139" s="2"/>
       <c r="C139" s="1" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>296</v>
+        <v>369</v>
       </c>
       <c r="B140" s="2"/>
       <c r="C140" s="1" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" s="1" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" s="1" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" s="1" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" s="1" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" s="1" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="B146" s="2"/>
       <c r="C146" s="1" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>319</v>
+        <v>371</v>
       </c>
       <c r="B147" s="2"/>
       <c r="C147" s="1" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>321</v>
+        <v>372</v>
       </c>
       <c r="B148" s="2"/>
       <c r="C148" s="1" t="s">
-        <v>322</v>
+        <v>303</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>323</v>
+        <v>374</v>
       </c>
       <c r="B149" s="2"/>
       <c r="C149" s="1" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>325</v>
+        <v>373</v>
       </c>
       <c r="B150" s="2"/>
       <c r="C150" s="1" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>327</v>
+        <v>306</v>
       </c>
       <c r="B151" s="2"/>
       <c r="C151" s="1" t="s">
-        <v>328</v>
+        <v>307</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>330</v>
+        <v>375</v>
       </c>
       <c r="B152" s="2"/>
       <c r="C152" s="1" t="s">
-        <v>331</v>
+        <v>309</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>323</v>
+        <v>374</v>
       </c>
       <c r="B153" s="2"/>
       <c r="C153" s="1" t="s">
-        <v>332</v>
+        <v>310</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>333</v>
+        <v>377</v>
       </c>
       <c r="B154" s="2"/>
       <c r="C154" s="1" t="s">
-        <v>334</v>
+        <v>311</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>335</v>
+        <v>376</v>
       </c>
       <c r="B155" s="2"/>
       <c r="C155" s="1" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>337</v>
+        <v>313</v>
       </c>
       <c r="B156" s="2"/>
       <c r="C156" s="1" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="B158" s="2"/>
       <c r="C158" s="1" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="B159" s="2"/>
       <c r="C159" s="1" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" s="1" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
       <c r="B161" s="2"/>
       <c r="C161" s="1" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" s="1" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" s="1" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" s="1" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" s="1" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve the translation naming of variables
</commit_message>
<xml_diff>
--- a/Conversion-Script/Variable_Reference/Variable_name_IAMC.xlsx
+++ b/Conversion-Script/Variable_Reference/Variable_name_IAMC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdGeeds\Documents\IAMC-format\IAMC_format\Conversion-Script\Variable_Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1926A5-0C12-43C3-972E-16C38F466808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07D2F50-C24E-4C57-B645-925DEB098693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="387">
   <si>
     <t>IAMC_variable</t>
   </si>
@@ -537,15 +537,9 @@
     <t>consumption_COICOP_real</t>
   </si>
   <si>
-    <t>Final Demand|Imports|Basic prices|Components</t>
-  </si>
-  <si>
     <t>final_demand_imports_in_basic_prices_real_by_component</t>
   </si>
   <si>
-    <t>Final Demand|Domestic|Basic prices|Components</t>
-  </si>
-  <si>
     <t>final_demand_dometic_in_basic_prices_real_by_component</t>
   </si>
   <si>
@@ -1053,9 +1047,6 @@
     <t>relative_RURR_Fe</t>
   </si>
   <si>
-    <t>Energy|Supply|Storage|Losses Vs Transformation Output [Share]</t>
-  </si>
-  <si>
     <t>Capacity|Electricity</t>
   </si>
   <si>
@@ -1068,24 +1059,9 @@
     <t>Revenue|Government</t>
   </si>
   <si>
-    <t>Primary Energy|Renewable [Share]</t>
-  </si>
-  <si>
-    <t>Final Energy|Renewable [Share]</t>
-  </si>
-  <si>
-    <t>Final Energy|Electricity|Renewable [Share]</t>
-  </si>
-  <si>
-    <t>Households|Consumer Price [index]</t>
-  </si>
-  <si>
     <t>Value Added|Net Operating Surplus</t>
   </si>
   <si>
-    <t>Population|Urban [Share]</t>
-  </si>
-  <si>
     <t>Final Energy|Transportation|Smart Charging|Electricity</t>
   </si>
   <si>
@@ -1098,9 +1074,6 @@
     <t>Price Adjusted|Primary Energy</t>
   </si>
   <si>
-    <t>Primary Energy|Commodity</t>
-  </si>
-  <si>
     <t>Sea level|Regional Mean rise</t>
   </si>
   <si>
@@ -1189,13 +1162,37 @@
   </si>
   <si>
     <t>Primary Energy Intensity|GDP[Annual change]</t>
+  </si>
+  <si>
+    <t>Population|Urban[Share]</t>
+  </si>
+  <si>
+    <t>Households|Consumer Price[index]</t>
+  </si>
+  <si>
+    <t>Final Energy|Electricity|Renewable[Share]</t>
+  </si>
+  <si>
+    <t>Final Energy|Renewable[Share]</t>
+  </si>
+  <si>
+    <t>Primary Energy|Renewable[Share]</t>
+  </si>
+  <si>
+    <t>Energy|Supply|Storage|Losses Vs Transformation Output[Share]</t>
+  </si>
+  <si>
+    <t>Final Demand|Imports|Basic prices</t>
+  </si>
+  <si>
+    <t>Final Demand|Domestic|Basic prices</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1206,6 +1203,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1234,7 +1238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1248,6 +1252,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1566,8 +1573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1629,7 +1636,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
@@ -1641,7 +1648,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
@@ -1719,7 +1726,7 @@
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>31</v>
@@ -1733,7 +1740,7 @@
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>31</v>
@@ -1761,7 +1768,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>38</v>
@@ -1985,7 +1992,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>64</v>
@@ -1999,7 +2006,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>64</v>
@@ -2013,7 +2020,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>352</v>
+        <v>379</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>81</v>
@@ -2139,7 +2146,7 @@
     </row>
     <row r="42" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>84</v>
@@ -2349,7 +2356,7 @@
     </row>
     <row r="57" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>84</v>
@@ -2363,7 +2370,7 @@
     </row>
     <row r="58" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>84</v>
@@ -2503,7 +2510,7 @@
     </row>
     <row r="68" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>84</v>
@@ -2517,7 +2524,7 @@
     </row>
     <row r="69" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>84</v>
@@ -2531,7 +2538,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>350</v>
+        <v>380</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>81</v>
@@ -2545,7 +2552,7 @@
     </row>
     <row r="71" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>84</v>
@@ -2559,7 +2566,7 @@
     </row>
     <row r="72" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>84</v>
@@ -2573,7 +2580,7 @@
     </row>
     <row r="73" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>84</v>
@@ -2587,7 +2594,7 @@
     </row>
     <row r="74" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>84</v>
@@ -2601,7 +2608,7 @@
     </row>
     <row r="75" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>84</v>
@@ -2629,7 +2636,7 @@
     </row>
     <row r="77" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>84</v>
@@ -2643,13 +2650,13 @@
     </row>
     <row r="78" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>164</v>
@@ -2657,13 +2664,13 @@
     </row>
     <row r="79" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>172</v>
+        <v>386</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>164</v>
@@ -2671,77 +2678,77 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>13</v>
@@ -2749,11 +2756,11 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>13</v>
@@ -2761,23 +2768,23 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>13</v>
@@ -2785,119 +2792,119 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>349</v>
+        <v>381</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>13</v>
@@ -2905,13 +2912,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>348</v>
+        <v>382</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -2919,13 +2926,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>347</v>
+        <v>383</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>13</v>
@@ -2933,39 +2940,39 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="D100" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>342</v>
+      <c r="A102" s="7" t="s">
+        <v>384</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>13</v>
@@ -2973,55 +2980,55 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="D103" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>164</v>
@@ -3029,13 +3036,13 @@
     </row>
     <row r="107" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>164</v>
@@ -3043,13 +3050,13 @@
     </row>
     <row r="108" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>164</v>
@@ -3057,13 +3064,13 @@
     </row>
     <row r="109" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>164</v>
@@ -3071,13 +3078,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>13</v>
@@ -3085,13 +3092,13 @@
     </row>
     <row r="111" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>164</v>
@@ -3099,11 +3106,11 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>13</v>
@@ -3111,23 +3118,23 @@
     </row>
     <row r="113" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>13</v>
@@ -3135,11 +3142,11 @@
     </row>
     <row r="115" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>13</v>
@@ -3147,23 +3154,23 @@
     </row>
     <row r="116" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>13</v>
@@ -3171,11 +3178,11 @@
     </row>
     <row r="118" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>13</v>
@@ -3183,225 +3190,225 @@
     </row>
     <row r="119" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="6" t="s">
-        <v>357</v>
+      <c r="A121" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B121" s="2"/>
       <c r="C121" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D121" s="2"/>
     </row>
     <row r="122" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="B122" s="2"/>
       <c r="C122" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="B124" s="2"/>
       <c r="C124" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B126" s="4"/>
       <c r="C126" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B130" s="2"/>
       <c r="C130" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B131" s="2"/>
       <c r="C131" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B132" s="2"/>
       <c r="C132" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B133" s="2"/>
       <c r="C133" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B136" s="2"/>
       <c r="C136" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B137" s="2"/>
       <c r="C137" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>13</v>
@@ -3409,119 +3416,119 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="B138" s="2"/>
       <c r="C138" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="B139" s="2"/>
       <c r="C139" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="B140" s="2"/>
       <c r="C140" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B146" s="2"/>
       <c r="C146" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="B147" s="2"/>
       <c r="C147" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>13</v>
@@ -3529,11 +3536,11 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B148" s="2"/>
       <c r="C148" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>13</v>
@@ -3541,11 +3548,11 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="B149" s="2"/>
       <c r="C149" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>13</v>
@@ -3553,11 +3560,11 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="B150" s="2"/>
       <c r="C150" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>13</v>
@@ -3565,23 +3572,23 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B151" s="2"/>
       <c r="C151" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="B152" s="2"/>
       <c r="C152" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>13</v>
@@ -3589,11 +3596,11 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="B153" s="2"/>
       <c r="C153" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>13</v>
@@ -3601,11 +3608,11 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="B154" s="2"/>
       <c r="C154" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>13</v>
@@ -3613,11 +3620,11 @@
     </row>
     <row r="155" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="B155" s="2"/>
       <c r="C155" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>13</v>
@@ -3625,149 +3632,149 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B156" s="2"/>
       <c r="C156" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C157" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B157" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="D157" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B158" s="2"/>
       <c r="C158" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B159" s="2"/>
       <c r="C159" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="B161" s="2"/>
       <c r="C161" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C164" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="B164" s="1" t="s">
+      <c r="D164" s="1" t="s">
         <v>333</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
update script to have the correct naming
</commit_message>
<xml_diff>
--- a/Conversion-Script/Variable_Reference/Variable_name_IAMC.xlsx
+++ b/Conversion-Script/Variable_Reference/Variable_name_IAMC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdGeeds\Documents\IAMC-format\IAMC_format\Conversion-Script\Variable_Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45688D7C-4114-42F6-B6F2-8DD52D55B82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C4A0A7-0797-46DE-B559-805B868AA6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-5050" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="413">
   <si>
     <t>IAMC_variable</t>
   </si>
@@ -450,9 +450,6 @@
     <t>government_debt</t>
   </si>
   <si>
-    <t>Revenues|Households|Disposable income</t>
-  </si>
-  <si>
     <t>DB_HH_DISPOSABLE_INCOME</t>
   </si>
   <si>
@@ -468,9 +465,6 @@
     <t>DB_HH_SAVINGS</t>
   </si>
   <si>
-    <t>Revenues|Households|Disposable income|Nominal</t>
-  </si>
-  <si>
     <t>disposable_income</t>
   </si>
   <si>
@@ -699,9 +693,6 @@
     <t>investment_cost_PROFLEX</t>
   </si>
   <si>
-    <t>Capital Cost|Energy Supply|Electricity|Flexibility </t>
-  </si>
-  <si>
     <t>total_PROFLEX_investment_cost</t>
   </si>
   <si>
@@ -1137,9 +1128,6 @@
     <t>Production Potential|Remaining|Heat</t>
   </si>
   <si>
-    <t>Capacity Additions|FlexibilityRequirements|Electricity</t>
-  </si>
-  <si>
     <t>Primary Energy Intensity GDP</t>
   </si>
   <si>
@@ -1164,12 +1152,6 @@
     <t>Emissions|CO2|Land Use Changes</t>
   </si>
   <si>
-    <t>Sea level|Regional Mean Rise</t>
-  </si>
-  <si>
-    <t>Sea level|Global Mean Rise</t>
-  </si>
-  <si>
     <t>final_energy_substitution_component</t>
   </si>
   <si>
@@ -1207,6 +1189,90 @@
   </si>
   <si>
     <t>Resource Reserve Production|Iron[ratio]</t>
+  </si>
+  <si>
+    <t>Revenues|Households|Disposable Income</t>
+  </si>
+  <si>
+    <t>Sea Level|Regional Mean Rise</t>
+  </si>
+  <si>
+    <t>Sea Level|Global Mean Rise</t>
+  </si>
+  <si>
+    <t>Revenues|Households|Disposable Income|Nominal</t>
+  </si>
+  <si>
+    <t>factor_of_minimum_land_limit</t>
+  </si>
+  <si>
+    <t>share_solar_urban</t>
+  </si>
+  <si>
+    <t>share_required_embodied_FE_materials_BU_vs_PE_total</t>
+  </si>
+  <si>
+    <t>Lest</t>
+  </si>
+  <si>
+    <t>The</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Yest</t>
+  </si>
+  <si>
+    <t>required_embodied_FE_materials_BU</t>
+  </si>
+  <si>
+    <t>FEnUst_PROSTO_elec_dedicated</t>
+  </si>
+  <si>
+    <t>Yeste</t>
+  </si>
+  <si>
+    <t>Total_dynFEnU_PROTRA</t>
+  </si>
+  <si>
+    <t>Yester</t>
+  </si>
+  <si>
+    <t>physical_energy_intensity_TPE_vs_net_energy_uses</t>
+  </si>
+  <si>
+    <t>Yestery</t>
+  </si>
+  <si>
+    <t>Capital Cost|Energy Supply|Electricity|Flexibility</t>
+  </si>
+  <si>
+    <t>Yesteryp</t>
+  </si>
+  <si>
+    <t>Yesterypa</t>
+  </si>
+  <si>
+    <t>Yesterypar</t>
+  </si>
+  <si>
+    <t>energy_efficiency_component</t>
+  </si>
+  <si>
+    <t>final_non_energy_demand_by_FE_9R</t>
+  </si>
+  <si>
+    <t>final_to_primary_energy_by_region</t>
+  </si>
+  <si>
+    <t>consumption_COICOP</t>
+  </si>
+  <si>
+    <t>Yesterypart</t>
+  </si>
+  <si>
+    <t>Capacity Additions|Flexibility Requirements|Electricity</t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1268,6 +1334,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1582,10 +1649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D169"/>
+  <dimension ref="A1:D180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A159" sqref="A159"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1647,7 +1714,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
@@ -1659,7 +1726,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
@@ -1737,7 +1804,7 @@
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>31</v>
@@ -1751,7 +1818,7 @@
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>31</v>
@@ -1779,7 +1846,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>38</v>
@@ -1793,7 +1860,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>38</v>
@@ -1807,7 +1874,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>41</v>
@@ -1835,7 +1902,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>46</v>
@@ -1947,7 +2014,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>61</v>
@@ -2003,7 +2070,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>61</v>
@@ -2017,7 +2084,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>61</v>
@@ -2031,7 +2098,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>77</v>
@@ -2157,7 +2224,7 @@
     </row>
     <row r="42" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>80</v>
@@ -2367,7 +2434,7 @@
     </row>
     <row r="57" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>80</v>
@@ -2381,7 +2448,7 @@
     </row>
     <row r="58" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>80</v>
@@ -2437,13 +2504,13 @@
     </row>
     <row r="62" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>82</v>
@@ -2451,13 +2518,13 @@
     </row>
     <row r="63" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>82</v>
@@ -2465,13 +2532,13 @@
     </row>
     <row r="64" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>82</v>
@@ -2479,83 +2546,83 @@
     </row>
     <row r="65" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>13</v>
@@ -2563,213 +2630,213 @@
     </row>
     <row r="71" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D82" s="1"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>13</v>
@@ -2777,11 +2844,11 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>13</v>
@@ -2789,23 +2856,23 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>13</v>
@@ -2813,119 +2880,119 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>13</v>
@@ -2933,13 +3000,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>13</v>
@@ -2947,227 +3014,227 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="A101" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="B101" s="6"/>
+      <c r="C101" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="D102" s="1" t="s">
-        <v>13</v>
+        <v>194</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="B103" s="2"/>
+        <v>203</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>201</v>
+      </c>
       <c r="C103" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>209</v>
-      </c>
+        <v>360</v>
+      </c>
+      <c r="B104" s="2"/>
       <c r="C104" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>15</v>
+        <v>207</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>323</v>
+        <v>210</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>215</v>
+        <v>320</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>216</v>
+        <v>15</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>160</v>
+        <v>194</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C110" s="1" t="s">
+      <c r="D112" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D110" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+      <c r="B113" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C111" s="1" t="s">
+      <c r="D113" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B113" s="2"/>
-      <c r="C113" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>368</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>230</v>
+        <v>13</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>386</v>
+        <v>364</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>13</v>
+        <v>227</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>13</v>
@@ -3175,35 +3242,35 @@
     </row>
     <row r="117" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>385</v>
+        <v>365</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>13</v>
@@ -3211,357 +3278,357 @@
     </row>
     <row r="120" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>335</v>
+        <v>366</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>237</v>
+        <v>13</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B121" s="2"/>
       <c r="C121" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="3" t="s">
-        <v>4</v>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>333</v>
       </c>
       <c r="B122" s="2"/>
       <c r="C122" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D122" s="2"/>
-    </row>
-    <row r="123" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>337</v>
+        <v>235</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>237</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="D123" s="2"/>
     </row>
     <row r="124" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B124" s="2"/>
       <c r="C124" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B126" s="2"/>
       <c r="C126" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B127" s="2"/>
+      <c r="C127" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B128" s="4"/>
+      <c r="C128" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="D126" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A127" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="B127" s="4"/>
-      <c r="C127" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="B128" s="2"/>
-      <c r="C128" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>248</v>
+      <c r="D128" s="3" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>249</v>
+        <v>327</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" s="1" t="s">
-        <v>16</v>
+        <v>244</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B130" s="2"/>
       <c r="C130" s="1" t="s">
-        <v>251</v>
+        <v>16</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>388</v>
+        <v>247</v>
       </c>
       <c r="B131" s="2"/>
       <c r="C131" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="B132" s="2"/>
       <c r="C132" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>255</v>
+        <v>194</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>256</v>
+        <v>383</v>
       </c>
       <c r="B133" s="2"/>
       <c r="C133" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>365</v>
+        <v>255</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>182</v>
+        <v>252</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B136" s="2"/>
       <c r="C136" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B137" s="2"/>
       <c r="C137" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>263</v>
+        <v>412</v>
       </c>
       <c r="B138" s="2"/>
       <c r="C138" s="1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>13</v>
+        <v>209</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>342</v>
+        <v>260</v>
       </c>
       <c r="B139" s="2"/>
       <c r="C139" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>266</v>
+        <v>13</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B140" s="2"/>
       <c r="C140" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>271</v>
+        <v>339</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" s="1" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" s="1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B146" s="2"/>
       <c r="C146" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B147" s="2"/>
       <c r="C147" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>344</v>
+        <v>281</v>
       </c>
       <c r="B148" s="2"/>
       <c r="C148" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>13</v>
+        <v>278</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B149" s="2"/>
       <c r="C149" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>13</v>
@@ -3569,11 +3636,11 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B150" s="2"/>
       <c r="C150" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>13</v>
@@ -3581,11 +3648,11 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B151" s="2"/>
       <c r="C151" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>13</v>
@@ -3593,35 +3660,35 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>290</v>
+        <v>343</v>
       </c>
       <c r="B152" s="2"/>
       <c r="C152" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>292</v>
+        <v>13</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>348</v>
+        <v>287</v>
       </c>
       <c r="B153" s="2"/>
       <c r="C153" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>13</v>
+        <v>289</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B154" s="2"/>
       <c r="C154" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>13</v>
@@ -3629,188 +3696,290 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="B155" s="2"/>
       <c r="C155" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B156" s="2"/>
       <c r="C156" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>297</v>
+        <v>346</v>
       </c>
       <c r="B157" s="2"/>
       <c r="C157" s="1" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>276</v>
+        <v>13</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>300</v>
-      </c>
+        <v>294</v>
+      </c>
+      <c r="B158" s="2"/>
       <c r="C158" s="1" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="B159" s="1"/>
+        <v>296</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>297</v>
+      </c>
       <c r="C159" s="1" t="s">
-        <v>372</v>
+        <v>298</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>13</v>
+        <v>278</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="B160" s="2"/>
-      <c r="C160" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>281</v>
-      </c>
+      <c r="A160" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="B160" s="6"/>
+      <c r="C160" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="D160" s="1"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B161" s="2"/>
+        <v>369</v>
+      </c>
+      <c r="B161" s="1"/>
       <c r="C161" s="1" t="s">
-        <v>304</v>
+        <v>368</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>305</v>
+        <v>13</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>306</v>
+        <v>374</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" s="1" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" s="1" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="B164" s="2"/>
       <c r="C164" s="1" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>390</v>
+        <v>335</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>315</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="B166" s="2"/>
       <c r="C166" s="1" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>318</v>
+        <v>384</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" s="1" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B168" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="5" t="s">
-        <v>374</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" s="1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D169" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="B171" s="2"/>
+      <c r="C171" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D171" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="B172" s="7"/>
+      <c r="C172" s="7" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="B173" s="7"/>
+      <c r="C173" s="7" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="B174" s="7"/>
+      <c r="C174" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="B175" s="7"/>
+      <c r="C175" s="6" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="B176" s="7"/>
+      <c r="C176" s="6" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="B177" s="7"/>
+      <c r="C177" s="7" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="B178" s="7"/>
+      <c r="C178" s="7" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="B179" s="7"/>
+      <c r="C179" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="C180" s="6" t="s">
+        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>